<commit_message>
updated exel file with news titles
</commit_message>
<xml_diff>
--- a/src/test/java/pl/com/interia/contentTest/News.xlsx
+++ b/src/test/java/pl/com/interia/contentTest/News.xlsx
@@ -16,31 +16,31 @@
     <t>NEWS</t>
   </si>
   <si>
-    <t>Lewandowski wrócił z przytupem! Zdobył bramkę po zawieszeniu!</t>
-  </si>
-  <si>
-    <t>"Podatek od zrzutek". Premier zapowiada ważne zmiany</t>
-  </si>
-  <si>
-    <t>Analityk wojenny: To może być największa pomyłka Ukraińców</t>
-  </si>
-  <si>
-    <t>"Rosja przygotowuje dużą ofensywę". Padła data</t>
-  </si>
-  <si>
-    <t>"Lewy" wrócił i strzelił! Kluczowy gol Polaka. Zobacz, jak "dobił" rywala</t>
-  </si>
-  <si>
-    <t>Pożar w ogromnej piekarni na Mazowszu. Ewakuowano ponad 200 osób</t>
-  </si>
-  <si>
-    <t>Zapadła decyzja w sprawie stóp procentowych w USA</t>
-  </si>
-  <si>
-    <t>Ostra reakcja ws. Rosji i Białorusi. Pierwszy kraj grozi bojkotem igrzysk</t>
-  </si>
-  <si>
-    <t>Wielka gwiazda znów odwiedzi Polskę! Czekaliśmy kilka lat</t>
+    <t>Gigantyczna lawina w rejonie Morskiego Oka. Jest nagranie</t>
+  </si>
+  <si>
+    <t>Ulubiony klub jachtowy Rosjan w płomieniach</t>
+  </si>
+  <si>
+    <t>Problemy w Willingen! Polacy poradzą sobie w kwalifikacjach?</t>
+  </si>
+  <si>
+    <t>Media: Reznikow straci stanowisko. Podano nazwisko następcy</t>
+  </si>
+  <si>
+    <t>Depardieu: Dla mnie nic się nie zmieniło. Nadal jestem Rosjaninem</t>
+  </si>
+  <si>
+    <t>Politycy odpowiadają premierowi. Czarzasty: Małpie brzytwy się nie daje</t>
+  </si>
+  <si>
+    <t>Patrioty zmierzają do Warszawy. Zostaną rozstawione na lotnisku</t>
+  </si>
+  <si>
+    <t>Te osoby mogą podwyższyć sobie emeryturę. Wystarczy jeden wniosek</t>
+  </si>
+  <si>
+    <t>Filmowe tytuły, z których śmieją się wszyscy. Kto je wybiera?</t>
   </si>
 </sst>
 </file>

</xml_diff>